<commit_message>
Everything must be ok
</commit_message>
<xml_diff>
--- a/photos_to_save.xlsx
+++ b/photos_to_save.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[{'height': 72, 'type': 'm', 'width': 130, 'url': 'https://sun6-20.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=130x72&amp;quality=96&amp;sign=c84949ae63696355d76dc23e848bb385&amp;c_uniq_tag=QOr9KARW5D7r2CH9-VN5O8xbBVdRWSWM5AzVTEUzgZs&amp;type=album'}, {'height': 87, 'type': 'o', 'width': 130, 'url': 'https://sun6-20.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=130x87&amp;quality=96&amp;crop=35,0,354,237&amp;sign=1c6bc543c4e9076de6f3576c29d351df&amp;c_uniq_tag=DA8jsBL1GYy8EVRUQP0ACZGdLIZCM3gzplwJiAB2YHE&amp;type=album'}, {'height': 133, 'type': 'p', 'width': 200, 'url': 'https://sun6-20.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=200x133&amp;quality=96&amp;crop=34,0,356,237&amp;sign=ce0833673c0c7e3745cc8c4c96fbbb05&amp;c_uniq_tag=4qYBNECQO1MPntpZWMXRTf2TfgLTvnREM5YYxFBILUs&amp;type=album'}, {'height': 213, 'type': 'q', 'width': 320, 'url': 'https://sun6-20.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=320x213&amp;quality=96&amp;crop=34,0,356,237&amp;sign=5a0eff4ed8b654e29dbf7a24ab04d99c&amp;c_uniq_tag=IxAM0qCI7miir9Swjq8wPNWmGTEMGXD_TEp13_q5oJc&amp;type=album'}, {'height': 237, 'type': 'r', 'width': 425, 'url': 'https://sun6-20.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=425x237&amp;quality=96&amp;sign=8b341f05c8a5cf6ccea8d1b6fad298c3&amp;c_uniq_tag=XGZXBEF_lHOI-jN1YPRuOExzRi1D9BRs9pRar7oVc8U&amp;type=album'}, {'height': 42, 'type': 's', 'width': 75, 'url': 'https://sun6-20.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=75x42&amp;quality=96&amp;sign=2f56e2b27cde273a07dc0b89d44d328e&amp;c_uniq_tag=2eLosGiatbQapxr5PlkwdTscCR8SKlHR7JAowK8NzrQ&amp;type=album'}, {'height': 237, 'type': 'x', 'width': 425, 'url': 'https://sun6-20.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=425x237&amp;quality=96&amp;sign=8b341f05c8a5cf6ccea8d1b6fad298c3&amp;c_uniq_tag=XGZXBEF_lHOI-jN1YPRuOExzRi1D9BRs9pRar7oVc8U&amp;type=album'}]</t>
+          <t>[{'height': 72, 'type': 'm', 'width': 130, 'url': 'https://sun9-80.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=130x72&amp;quality=96&amp;sign=c84949ae63696355d76dc23e848bb385&amp;c_uniq_tag=QOr9KARW5D7r2CH9-VN5O8xbBVdRWSWM5AzVTEUzgZs&amp;type=album'}, {'height': 87, 'type': 'o', 'width': 130, 'url': 'https://sun9-80.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=130x87&amp;quality=96&amp;crop=35,0,354,237&amp;sign=1c6bc543c4e9076de6f3576c29d351df&amp;c_uniq_tag=DA8jsBL1GYy8EVRUQP0ACZGdLIZCM3gzplwJiAB2YHE&amp;type=album'}, {'height': 133, 'type': 'p', 'width': 200, 'url': 'https://sun9-80.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=200x133&amp;quality=96&amp;crop=34,0,356,237&amp;sign=ce0833673c0c7e3745cc8c4c96fbbb05&amp;c_uniq_tag=4qYBNECQO1MPntpZWMXRTf2TfgLTvnREM5YYxFBILUs&amp;type=album'}, {'height': 213, 'type': 'q', 'width': 320, 'url': 'https://sun9-80.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=320x213&amp;quality=96&amp;crop=34,0,356,237&amp;sign=5a0eff4ed8b654e29dbf7a24ab04d99c&amp;c_uniq_tag=IxAM0qCI7miir9Swjq8wPNWmGTEMGXD_TEp13_q5oJc&amp;type=album'}, {'height': 237, 'type': 'r', 'width': 425, 'url': 'https://sun9-80.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=425x237&amp;quality=96&amp;sign=8b341f05c8a5cf6ccea8d1b6fad298c3&amp;c_uniq_tag=XGZXBEF_lHOI-jN1YPRuOExzRi1D9BRs9pRar7oVc8U&amp;type=album'}, {'height': 42, 'type': 's', 'width': 75, 'url': 'https://sun9-80.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=75x42&amp;quality=96&amp;sign=2f56e2b27cde273a07dc0b89d44d328e&amp;c_uniq_tag=2eLosGiatbQapxr5PlkwdTscCR8SKlHR7JAowK8NzrQ&amp;type=album'}, {'height': 237, 'type': 'x', 'width': 425, 'url': 'https://sun9-80.userapi.com/impf/Zod66xVvQ4LUlX9ifyGHz1o28F_XKBU-wERiCg/Ak_4vFJhIao.jpg?size=425x237&amp;quality=96&amp;sign=8b341f05c8a5cf6ccea8d1b6fad298c3&amp;c_uniq_tag=XGZXBEF_lHOI-jN1YPRuOExzRi1D9BRs9pRar7oVc8U&amp;type=album'}]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -697,7 +697,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[{'height': 75, 'type': 's', 'width': 65, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=65x75&amp;quality=95&amp;sign=8c1c7cbc9279728e86dac499b84d7178&amp;c_uniq_tag=himzbnkelzKUGdwFpGaphg61TVbef6UvKad41ohRF6w&amp;type=album'}, {'height': 130, 'type': 'm', 'width': 112, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=112x130&amp;quality=95&amp;sign=8bccc2efc9599fe91f37e2a93cac999b&amp;c_uniq_tag=WLmHViOkEn8klhI1k4jloOi7PJBVPeSba-8MN9HZKb0&amp;type=album'}, {'height': 604, 'type': 'x', 'width': 521, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=521x604&amp;quality=95&amp;sign=ba6910ef5ada5cba81f8bae534581e00&amp;c_uniq_tag=3hHlAyyUO-S7DpGBWcWVh9QsnZBD-MHxyWVtdnroifs&amp;type=album'}, {'height': 636, 'type': 'y', 'width': 549, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=549x636&amp;quality=95&amp;sign=c57b4756ac220f634b39f8c55718ad79&amp;c_uniq_tag=FaL4LW3Mg-HSlQi2c9Ne2DwMLGUDTbFGANrry8JcGyA&amp;type=album'}, {'height': 151, 'type': 'o', 'width': 130, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=130x151&amp;quality=95&amp;sign=528d7555b4295e6e9136e205a05e0fd3&amp;c_uniq_tag=NXd1aXNsh_f8S4L-18gSKEKJJVdkpTAC3957pQA-w5A&amp;type=album'}, {'height': 232, 'type': 'p', 'width': 200, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=200x232&amp;quality=95&amp;sign=0f2594ecc1406025e42b3115afc8d91a&amp;c_uniq_tag=UqeZksZ31x65nMQM3_RYVwMbkfXOxjQ6KBLubgNNQd4&amp;type=album'}, {'height': 371, 'type': 'q', 'width': 320, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=320x371&amp;quality=95&amp;sign=752bc01d316120b4a4ebef19bbb0df4c&amp;c_uniq_tag=yScDWtI0dcBYPK3qwvH7Frdb42dfqCtiJNAifCDlBTA&amp;type=album'}, {'height': 591, 'type': 'r', 'width': 510, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=510x591&amp;quality=95&amp;sign=0aeed757cae161429e40081314bde190&amp;c_uniq_tag=c3lRWixdUGXmsJzM0gTFlnLOlKFxoeruO83aV0OG__E&amp;type=album'}]</t>
+          <t>[{'height': 75, 'type': 's', 'width': 65, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=65x75&amp;quality=95&amp;sign=8c1c7cbc9279728e86dac499b84d7178&amp;c_uniq_tag=himzbnkelzKUGdwFpGaphg61TVbef6UvKad41ohRF6w&amp;type=album'}, {'height': 130, 'type': 'm', 'width': 112, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=112x130&amp;quality=95&amp;sign=8bccc2efc9599fe91f37e2a93cac999b&amp;c_uniq_tag=WLmHViOkEn8klhI1k4jloOi7PJBVPeSba-8MN9HZKb0&amp;type=album'}, {'height': 604, 'type': 'x', 'width': 521, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=521x604&amp;quality=95&amp;sign=ba6910ef5ada5cba81f8bae534581e00&amp;c_uniq_tag=3hHlAyyUO-S7DpGBWcWVh9QsnZBD-MHxyWVtdnroifs&amp;type=album'}, {'height': 636, 'type': 'y', 'width': 549, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=549x636&amp;quality=95&amp;sign=c57b4756ac220f634b39f8c55718ad79&amp;c_uniq_tag=FaL4LW3Mg-HSlQi2c9Ne2DwMLGUDTbFGANrry8JcGyA&amp;type=album'}, {'height': 151, 'type': 'o', 'width': 130, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=130x151&amp;quality=95&amp;sign=528d7555b4295e6e9136e205a05e0fd3&amp;c_uniq_tag=NXd1aXNsh_f8S4L-18gSKEKJJVdkpTAC3957pQA-w5A&amp;type=album'}, {'height': 232, 'type': 'p', 'width': 200, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=200x232&amp;quality=95&amp;sign=0f2594ecc1406025e42b3115afc8d91a&amp;c_uniq_tag=UqeZksZ31x65nMQM3_RYVwMbkfXOxjQ6KBLubgNNQd4&amp;type=album'}, {'height': 371, 'type': 'q', 'width': 320, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=320x371&amp;quality=95&amp;sign=752bc01d316120b4a4ebef19bbb0df4c&amp;c_uniq_tag=yScDWtI0dcBYPK3qwvH7Frdb42dfqCtiJNAifCDlBTA&amp;type=album'}, {'height': 591, 'type': 'r', 'width': 510, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=510x591&amp;quality=95&amp;sign=0aeed757cae161429e40081314bde190&amp;c_uniq_tag=c3lRWixdUGXmsJzM0gTFlnLOlKFxoeruO83aV0OG__E&amp;type=album'}]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>

</xml_diff>

<commit_message>
all works and even fotos if exists on YaDisk do not doubles
</commit_message>
<xml_diff>
--- a/photos_to_save.xlsx
+++ b/photos_to_save.xlsx
@@ -651,7 +651,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[{'height': 75, 'type': 's', 'width': 72, 'url': 'https://sun6-22.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=72x75&amp;quality=95&amp;sign=ceadc6d93b394bd647d90a5417220fb7&amp;c_uniq_tag=-kCQ6BPt_tR8t7hXkMCCiHCjlay1oUD5l2o7cj5nCOA&amp;type=album'}, {'height': 130, 'type': 'm', 'width': 125, 'url': 'https://sun6-22.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=125x130&amp;quality=95&amp;sign=0c6e99634a50e17d9d397d6bd108a43e&amp;c_uniq_tag=Tw6-BjHxmToJ6E7w19MorkPonW0s5TgkgMidC4Hu5ZI&amp;type=album'}, {'height': 570, 'type': 'x', 'width': 548, 'url': 'https://sun6-22.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=548x570&amp;quality=95&amp;sign=9beb4b83c4bf56cd15e694da8dbe68a3&amp;c_uniq_tag=PeNLgrvRr3ik5WWJp7TdbPEkbBL9tsok_vbZ2PgbmgI&amp;type=album'}, {'height': 135, 'type': 'o', 'width': 130, 'url': 'https://sun6-22.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=130x135&amp;quality=95&amp;sign=bed5f01625b9acf1e809b8bf504a1568&amp;c_uniq_tag=NMPRKa_OZ1mMNu0PxfHhZeWvtndY_2v0ZRG1MoKJJ1s&amp;type=album'}, {'height': 208, 'type': 'p', 'width': 200, 'url': 'https://sun6-22.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=200x208&amp;quality=95&amp;sign=3ed6eff7be0a99403e1d881187404df3&amp;c_uniq_tag=TWWbNyJJveKoteJPj6juhvXmu94FarlhZxujw_bBGag&amp;type=album'}, {'height': 333, 'type': 'q', 'width': 320, 'url': 'https://sun6-22.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=320x333&amp;quality=95&amp;sign=44428fcbcb93aeba97a3845c001f4691&amp;c_uniq_tag=87pTBzsOmbPERGmw9mAw1Exg__tagnoctYl-dvRKjY4&amp;type=album'}, {'height': 530, 'type': 'r', 'width': 510, 'url': 'https://sun6-22.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=510x530&amp;quality=95&amp;sign=595ac79f507ef1450befd78e51e326e4&amp;c_uniq_tag=cB_FgSo5fgznzpL8J9EWIWReBR0jvr_iIrvVF86hXdA&amp;type=album'}]</t>
+          <t>[{'height': 75, 'type': 's', 'width': 72, 'url': 'https://sun9-1.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=72x75&amp;quality=95&amp;sign=ceadc6d93b394bd647d90a5417220fb7&amp;c_uniq_tag=-kCQ6BPt_tR8t7hXkMCCiHCjlay1oUD5l2o7cj5nCOA&amp;type=album'}, {'height': 130, 'type': 'm', 'width': 125, 'url': 'https://sun9-1.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=125x130&amp;quality=95&amp;sign=0c6e99634a50e17d9d397d6bd108a43e&amp;c_uniq_tag=Tw6-BjHxmToJ6E7w19MorkPonW0s5TgkgMidC4Hu5ZI&amp;type=album'}, {'height': 570, 'type': 'x', 'width': 548, 'url': 'https://sun9-1.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=548x570&amp;quality=95&amp;sign=9beb4b83c4bf56cd15e694da8dbe68a3&amp;c_uniq_tag=PeNLgrvRr3ik5WWJp7TdbPEkbBL9tsok_vbZ2PgbmgI&amp;type=album'}, {'height': 135, 'type': 'o', 'width': 130, 'url': 'https://sun9-1.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=130x135&amp;quality=95&amp;sign=bed5f01625b9acf1e809b8bf504a1568&amp;c_uniq_tag=NMPRKa_OZ1mMNu0PxfHhZeWvtndY_2v0ZRG1MoKJJ1s&amp;type=album'}, {'height': 208, 'type': 'p', 'width': 200, 'url': 'https://sun9-1.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=200x208&amp;quality=95&amp;sign=3ed6eff7be0a99403e1d881187404df3&amp;c_uniq_tag=TWWbNyJJveKoteJPj6juhvXmu94FarlhZxujw_bBGag&amp;type=album'}, {'height': 333, 'type': 'q', 'width': 320, 'url': 'https://sun9-1.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=320x333&amp;quality=95&amp;sign=44428fcbcb93aeba97a3845c001f4691&amp;c_uniq_tag=87pTBzsOmbPERGmw9mAw1Exg__tagnoctYl-dvRKjY4&amp;type=album'}, {'height': 530, 'type': 'r', 'width': 510, 'url': 'https://sun9-1.userapi.com/impg/R1GvQjpNBIemCtctu5z8wUEN3S3Rzs4ejo1iZA/ws9L6oc7-SI.jpg?size=510x530&amp;quality=95&amp;sign=595ac79f507ef1450befd78e51e326e4&amp;c_uniq_tag=cB_FgSo5fgznzpL8J9EWIWReBR0jvr_iIrvVF86hXdA&amp;type=album'}]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -697,7 +697,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[{'height': 75, 'type': 's', 'width': 65, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=65x75&amp;quality=95&amp;sign=8c1c7cbc9279728e86dac499b84d7178&amp;c_uniq_tag=himzbnkelzKUGdwFpGaphg61TVbef6UvKad41ohRF6w&amp;type=album'}, {'height': 130, 'type': 'm', 'width': 112, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=112x130&amp;quality=95&amp;sign=8bccc2efc9599fe91f37e2a93cac999b&amp;c_uniq_tag=WLmHViOkEn8klhI1k4jloOi7PJBVPeSba-8MN9HZKb0&amp;type=album'}, {'height': 604, 'type': 'x', 'width': 521, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=521x604&amp;quality=95&amp;sign=ba6910ef5ada5cba81f8bae534581e00&amp;c_uniq_tag=3hHlAyyUO-S7DpGBWcWVh9QsnZBD-MHxyWVtdnroifs&amp;type=album'}, {'height': 636, 'type': 'y', 'width': 549, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=549x636&amp;quality=95&amp;sign=c57b4756ac220f634b39f8c55718ad79&amp;c_uniq_tag=FaL4LW3Mg-HSlQi2c9Ne2DwMLGUDTbFGANrry8JcGyA&amp;type=album'}, {'height': 151, 'type': 'o', 'width': 130, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=130x151&amp;quality=95&amp;sign=528d7555b4295e6e9136e205a05e0fd3&amp;c_uniq_tag=NXd1aXNsh_f8S4L-18gSKEKJJVdkpTAC3957pQA-w5A&amp;type=album'}, {'height': 232, 'type': 'p', 'width': 200, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=200x232&amp;quality=95&amp;sign=0f2594ecc1406025e42b3115afc8d91a&amp;c_uniq_tag=UqeZksZ31x65nMQM3_RYVwMbkfXOxjQ6KBLubgNNQd4&amp;type=album'}, {'height': 371, 'type': 'q', 'width': 320, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=320x371&amp;quality=95&amp;sign=752bc01d316120b4a4ebef19bbb0df4c&amp;c_uniq_tag=yScDWtI0dcBYPK3qwvH7Frdb42dfqCtiJNAifCDlBTA&amp;type=album'}, {'height': 591, 'type': 'r', 'width': 510, 'url': 'https://sun6-23.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=510x591&amp;quality=95&amp;sign=0aeed757cae161429e40081314bde190&amp;c_uniq_tag=c3lRWixdUGXmsJzM0gTFlnLOlKFxoeruO83aV0OG__E&amp;type=album'}]</t>
+          <t>[{'height': 75, 'type': 's', 'width': 65, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=65x75&amp;quality=95&amp;sign=8c1c7cbc9279728e86dac499b84d7178&amp;c_uniq_tag=himzbnkelzKUGdwFpGaphg61TVbef6UvKad41ohRF6w&amp;type=album'}, {'height': 130, 'type': 'm', 'width': 112, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=112x130&amp;quality=95&amp;sign=8bccc2efc9599fe91f37e2a93cac999b&amp;c_uniq_tag=WLmHViOkEn8klhI1k4jloOi7PJBVPeSba-8MN9HZKb0&amp;type=album'}, {'height': 604, 'type': 'x', 'width': 521, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=521x604&amp;quality=95&amp;sign=ba6910ef5ada5cba81f8bae534581e00&amp;c_uniq_tag=3hHlAyyUO-S7DpGBWcWVh9QsnZBD-MHxyWVtdnroifs&amp;type=album'}, {'height': 636, 'type': 'y', 'width': 549, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=549x636&amp;quality=95&amp;sign=c57b4756ac220f634b39f8c55718ad79&amp;c_uniq_tag=FaL4LW3Mg-HSlQi2c9Ne2DwMLGUDTbFGANrry8JcGyA&amp;type=album'}, {'height': 151, 'type': 'o', 'width': 130, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=130x151&amp;quality=95&amp;sign=528d7555b4295e6e9136e205a05e0fd3&amp;c_uniq_tag=NXd1aXNsh_f8S4L-18gSKEKJJVdkpTAC3957pQA-w5A&amp;type=album'}, {'height': 232, 'type': 'p', 'width': 200, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=200x232&amp;quality=95&amp;sign=0f2594ecc1406025e42b3115afc8d91a&amp;c_uniq_tag=UqeZksZ31x65nMQM3_RYVwMbkfXOxjQ6KBLubgNNQd4&amp;type=album'}, {'height': 371, 'type': 'q', 'width': 320, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=320x371&amp;quality=95&amp;sign=752bc01d316120b4a4ebef19bbb0df4c&amp;c_uniq_tag=yScDWtI0dcBYPK3qwvH7Frdb42dfqCtiJNAifCDlBTA&amp;type=album'}, {'height': 591, 'type': 'r', 'width': 510, 'url': 'https://sun9-70.userapi.com/impg/4oEP1lzqDnKlVeAIpMuf-_drZY7qqK7negceug/EIJPzAzRttI.jpg?size=510x591&amp;quality=95&amp;sign=0aeed757cae161429e40081314bde190&amp;c_uniq_tag=c3lRWixdUGXmsJzM0gTFlnLOlKFxoeruO83aV0OG__E&amp;type=album'}]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>

</xml_diff>

<commit_message>
all works and made 2 classes instead 1
</commit_message>
<xml_diff>
--- a/photos_to_save.xlsx
+++ b/photos_to_save.xlsx
@@ -559,7 +559,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[{'height': 72, 'type': 'm', 'width': 130, 'url': 'https://sun6-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=130x72&amp;quality=96&amp;sign=978a0fd1e7b40fc893c2c496416368a2&amp;c_uniq_tag=zOpNgDtGLEtoplFgksOuP2_GBP171ue0YAzshaJdo5E&amp;type=album'}, {'height': 87, 'type': 'o', 'width': 130, 'url': 'https://sun6-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=130x87&amp;quality=96&amp;crop=35,0,354,237&amp;sign=7ea20a06e37b1dd4619006224142c7d3&amp;c_uniq_tag=7f0ZakCj1tlmnTMtawvjOEk4hRf19TA4VbMZPtl8OLA&amp;type=album'}, {'height': 133, 'type': 'p', 'width': 200, 'url': 'https://sun6-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=200x133&amp;quality=96&amp;crop=34,0,356,237&amp;sign=8a7a5283c6ddbc1229b327f7386bf7f2&amp;c_uniq_tag=wIzPNRQZHaWub2FWLOKI1KdCXOw9eq2LbYLC5A9Vvl8&amp;type=album'}, {'height': 213, 'type': 'q', 'width': 320, 'url': 'https://sun6-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=320x213&amp;quality=96&amp;crop=34,0,356,237&amp;sign=27d3671661ab5f1b42f7234c593e6efe&amp;c_uniq_tag=2-OfGh3UgI4kmuNiSxd-MnWOmGmdIb11_QaOv5Ld8O8&amp;type=album'}, {'height': 237, 'type': 'r', 'width': 425, 'url': 'https://sun6-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=425x237&amp;quality=96&amp;sign=c7ea5f719f2ad1bbebd03b4c09cb3b74&amp;c_uniq_tag=1q-FXm675FQHC8bgGEEhgonN_0UMsuMookqhsZZou4U&amp;type=album'}, {'height': 42, 'type': 's', 'width': 75, 'url': 'https://sun6-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=75x42&amp;quality=96&amp;sign=2c672725e67005bf85306faa2932913e&amp;c_uniq_tag=wIbrH2W5Wb-P3AE13unjtsbDYm_cdPqrRAY_o--cNkI&amp;type=album'}, {'height': 237, 'type': 'x', 'width': 425, 'url': 'https://sun6-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=425x237&amp;quality=96&amp;sign=c7ea5f719f2ad1bbebd03b4c09cb3b74&amp;c_uniq_tag=1q-FXm675FQHC8bgGEEhgonN_0UMsuMookqhsZZou4U&amp;type=album'}]</t>
+          <t>[{'height': 72, 'type': 'm', 'width': 130, 'url': 'https://sun9-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=130x72&amp;quality=96&amp;sign=978a0fd1e7b40fc893c2c496416368a2&amp;c_uniq_tag=zOpNgDtGLEtoplFgksOuP2_GBP171ue0YAzshaJdo5E&amp;type=album'}, {'height': 87, 'type': 'o', 'width': 130, 'url': 'https://sun9-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=130x87&amp;quality=96&amp;crop=35,0,354,237&amp;sign=7ea20a06e37b1dd4619006224142c7d3&amp;c_uniq_tag=7f0ZakCj1tlmnTMtawvjOEk4hRf19TA4VbMZPtl8OLA&amp;type=album'}, {'height': 133, 'type': 'p', 'width': 200, 'url': 'https://sun9-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=200x133&amp;quality=96&amp;crop=34,0,356,237&amp;sign=8a7a5283c6ddbc1229b327f7386bf7f2&amp;c_uniq_tag=wIzPNRQZHaWub2FWLOKI1KdCXOw9eq2LbYLC5A9Vvl8&amp;type=album'}, {'height': 213, 'type': 'q', 'width': 320, 'url': 'https://sun9-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=320x213&amp;quality=96&amp;crop=34,0,356,237&amp;sign=27d3671661ab5f1b42f7234c593e6efe&amp;c_uniq_tag=2-OfGh3UgI4kmuNiSxd-MnWOmGmdIb11_QaOv5Ld8O8&amp;type=album'}, {'height': 237, 'type': 'r', 'width': 425, 'url': 'https://sun9-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=425x237&amp;quality=96&amp;sign=c7ea5f719f2ad1bbebd03b4c09cb3b74&amp;c_uniq_tag=1q-FXm675FQHC8bgGEEhgonN_0UMsuMookqhsZZou4U&amp;type=album'}, {'height': 42, 'type': 's', 'width': 75, 'url': 'https://sun9-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=75x42&amp;quality=96&amp;sign=2c672725e67005bf85306faa2932913e&amp;c_uniq_tag=wIbrH2W5Wb-P3AE13unjtsbDYm_cdPqrRAY_o--cNkI&amp;type=album'}, {'height': 237, 'type': 'x', 'width': 425, 'url': 'https://sun9-21.userapi.com/impf/rVvupupMARwYPisPvjpqiRjy_Jedy5QkgOo9qQ/-SlMTPlXr-k.jpg?size=425x237&amp;quality=96&amp;sign=c7ea5f719f2ad1bbebd03b4c09cb3b74&amp;c_uniq_tag=1q-FXm675FQHC8bgGEEhgonN_0UMsuMookqhsZZou4U&amp;type=album'}]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -605,7 +605,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[{'height': 107, 'type': 'm', 'width': 130, 'url': 'https://sun6-23.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=130x107&amp;quality=96&amp;sign=6d40a77f971cf2c3724afdec8f12af19&amp;c_uniq_tag=7OEGfOssYHrQE4JK152VQHMMGE-1Xc8BkcD_mGeLIuA&amp;type=album'}, {'height': 107, 'type': 'o', 'width': 130, 'url': 'https://sun6-23.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=130x107&amp;quality=96&amp;sign=6d40a77f971cf2c3724afdec8f12af19&amp;c_uniq_tag=7OEGfOssYHrQE4JK152VQHMMGE-1Xc8BkcD_mGeLIuA&amp;type=album'}, {'height': 164, 'type': 'p', 'width': 200, 'url': 'https://sun6-23.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=200x164&amp;quality=96&amp;sign=ab446b6f06c4d2d46f4c1b7cd8ab5261&amp;c_uniq_tag=g7hNVGcS0liJNF5ht2vkmz8Oocux4CEF5rHiydD5EVA&amp;type=album'}, {'height': 263, 'type': 'q', 'width': 320, 'url': 'https://sun6-23.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=320x263&amp;quality=96&amp;sign=ee749c85514e7c9825a88a633b210b0d&amp;c_uniq_tag=VgJlmaNJ6129arzBRJhM2r4JJagg_j4fn5UtlXHyL5s&amp;type=album'}, {'height': 419, 'type': 'r', 'width': 510, 'url': 'https://sun6-23.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=510x419&amp;quality=96&amp;sign=34fc1dbd0260b7169a122b7fb2b79cf8&amp;c_uniq_tag=2njAdomZz4FKRur0BHgZmegZcDsTvFWMTa43IybIIwc&amp;type=album'}, {'height': 62, 'type': 's', 'width': 75, 'url': 'https://sun6-23.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=75x62&amp;quality=96&amp;sign=761c91142d1a23da8eb37b152cebc1dc&amp;c_uniq_tag=0oNbBbDW8gNroh8Dqg0h0fxd3dOfDlF6HJbvZQiJ8AI&amp;type=album'}, {'height': 458, 'type': 'x', 'width': 558, 'url': 'https://sun6-23.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=558x458&amp;quality=96&amp;sign=adabb4dd464586c3fed2957414b9b241&amp;c_uniq_tag=mnU8nhpZ7Mm1aqPQEcv3IsBq6Ftn0t8wsO_7wW1WIoM&amp;type=album'}]</t>
+          <t>[{'height': 107, 'type': 'm', 'width': 130, 'url': 'https://sun9-41.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=130x107&amp;quality=96&amp;sign=6d40a77f971cf2c3724afdec8f12af19&amp;c_uniq_tag=7OEGfOssYHrQE4JK152VQHMMGE-1Xc8BkcD_mGeLIuA&amp;type=album'}, {'height': 107, 'type': 'o', 'width': 130, 'url': 'https://sun9-41.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=130x107&amp;quality=96&amp;sign=6d40a77f971cf2c3724afdec8f12af19&amp;c_uniq_tag=7OEGfOssYHrQE4JK152VQHMMGE-1Xc8BkcD_mGeLIuA&amp;type=album'}, {'height': 164, 'type': 'p', 'width': 200, 'url': 'https://sun9-41.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=200x164&amp;quality=96&amp;sign=ab446b6f06c4d2d46f4c1b7cd8ab5261&amp;c_uniq_tag=g7hNVGcS0liJNF5ht2vkmz8Oocux4CEF5rHiydD5EVA&amp;type=album'}, {'height': 263, 'type': 'q', 'width': 320, 'url': 'https://sun9-41.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=320x263&amp;quality=96&amp;sign=ee749c85514e7c9825a88a633b210b0d&amp;c_uniq_tag=VgJlmaNJ6129arzBRJhM2r4JJagg_j4fn5UtlXHyL5s&amp;type=album'}, {'height': 419, 'type': 'r', 'width': 510, 'url': 'https://sun9-41.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=510x419&amp;quality=96&amp;sign=34fc1dbd0260b7169a122b7fb2b79cf8&amp;c_uniq_tag=2njAdomZz4FKRur0BHgZmegZcDsTvFWMTa43IybIIwc&amp;type=album'}, {'height': 62, 'type': 's', 'width': 75, 'url': 'https://sun9-41.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=75x62&amp;quality=96&amp;sign=761c91142d1a23da8eb37b152cebc1dc&amp;c_uniq_tag=0oNbBbDW8gNroh8Dqg0h0fxd3dOfDlF6HJbvZQiJ8AI&amp;type=album'}, {'height': 458, 'type': 'x', 'width': 558, 'url': 'https://sun9-41.userapi.com/impf/pXaQbeuh9ElsCBd93DGTPb4lSd1GybiInXXo2g/L8wErn2y2Hg.jpg?size=558x458&amp;quality=96&amp;sign=adabb4dd464586c3fed2957414b9b241&amp;c_uniq_tag=mnU8nhpZ7Mm1aqPQEcv3IsBq6Ftn0t8wsO_7wW1WIoM&amp;type=album'}]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>

</xml_diff>